<commit_message>
ccbottlersus fix templates and codes
</commit_message>
<xml_diff>
--- a/Projects/CCBOTTLERSUS_SAND/Data/KPITemplateV4.1.xlsx
+++ b/Projects/CCBOTTLERSUS_SAND/Data/KPITemplateV4.1.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="989" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="KPIs" sheetId="1" state="visible" r:id="rId2"/>
@@ -31,6 +31,8 @@
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">KPIs!$A$1:$Q$70</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0" vbProcedure="false">KPIs!$A$1:$Q$70</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">KPIs!$A$1:$Q$70</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0" vbProcedure="false">KPIs!$A$1:$Q$70</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0" vbProcedure="false">KPIs!$A$1:$Q$70</definedName>
     <definedName function="false" hidden="false" localSheetId="1" name="a" vbProcedure="false">Availability!$A$1:$J$64</definedName>
     <definedName function="false" hidden="false" localSheetId="1" name="b" vbProcedure="false">Availability!$A$1:$J$64</definedName>
     <definedName function="false" hidden="false" localSheetId="1" name="_FilterDatabase_0" vbProcedure="false">Availability!$A$1:$J$64</definedName>
@@ -41,6 +43,8 @@
     <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase" vbProcedure="false">Availability!$A$1:$J$64</definedName>
     <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0" vbProcedure="false">Availability!$A$1:$J$64</definedName>
     <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">Availability!$A$1:$J$64</definedName>
+    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0" vbProcedure="false">Availability!$A$1:$J$64</definedName>
+    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0_0" vbProcedure="false">Availability!$A$1:$J$64</definedName>
     <definedName function="false" hidden="false" localSheetId="3" name="a" vbProcedure="false">SOS!$A$1:$I$9</definedName>
     <definedName function="false" hidden="false" localSheetId="3" name="b" vbProcedure="false">SOS!$A$1:$I$9</definedName>
     <definedName function="false" hidden="false" localSheetId="3" name="_FilterDatabase_0" vbProcedure="false">SOS!$A$1:$I$9</definedName>
@@ -51,6 +55,8 @@
     <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase" vbProcedure="false">SOS!$A$1:$I$9</definedName>
     <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0" vbProcedure="false">SOS!$A$1:$I$9</definedName>
     <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">SOS!$A$1:$I$9</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0" vbProcedure="false">SOS!$A$1:$I$9</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0" vbProcedure="false">SOS!$A$1:$I$9</definedName>
     <definedName function="false" hidden="false" localSheetId="4" name="a" vbProcedure="false">Survey!$A$1:$E$24</definedName>
     <definedName function="false" hidden="false" localSheetId="4" name="b" vbProcedure="false">Survey!$A$1:$E$24</definedName>
     <definedName function="false" hidden="false" localSheetId="4" name="_FilterDatabase_0" vbProcedure="false">Survey!$A$1:$E$24</definedName>
@@ -61,6 +67,8 @@
     <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase" vbProcedure="false">Survey!$A$1:$E$24</definedName>
     <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0" vbProcedure="false">Survey!$A$1:$E$24</definedName>
     <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">Survey!$A$1:$E$24</definedName>
+    <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0_0_0" vbProcedure="false">Survey!$A$1:$E$24</definedName>
+    <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0_0_0_0" vbProcedure="false">Survey!$A$1:$E$24</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -72,7 +80,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1092" uniqueCount="282">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1084" uniqueCount="281">
   <si>
     <t>Region</t>
   </si>
@@ -750,9 +758,6 @@
   </si>
   <si>
     <t>att2</t>
-  </si>
-  <si>
-    <t>Powerade</t>
   </si>
   <si>
     <t>42.2, 42.25, 67, 67.6, 67.62, 68</t>
@@ -1321,20 +1326,20 @@
   </sheetPr>
   <dimension ref="A1:Q70"/>
   <sheetViews>
-    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="G2" activePane="bottomRight" state="frozen"/>
+    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="3" ySplit="1" topLeftCell="D26" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="G1" activeCellId="0" sqref="G1"/>
-      <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="L4" activeCellId="0" sqref="L4"/>
+      <selection pane="topRight" activeCell="D1" activeCellId="0" sqref="D1"/>
+      <selection pane="bottomLeft" activeCell="A26" activeCellId="0" sqref="A26"/>
+      <selection pane="bottomRight" activeCell="D34" activeCellId="0" sqref="D34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
     <col collapsed="false" hidden="false" max="3" min="1" style="1" width="8.67611336032389"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="23.2429149797571"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="23.0323886639676"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="37.7044534412955"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="23.4574898785425"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="23.2429149797571"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="38.2429149797571"/>
     <col collapsed="false" hidden="false" max="11" min="7" style="1" width="8.67611336032389"/>
     <col collapsed="false" hidden="false" max="12" min="12" style="1" width="13.9271255060729"/>
     <col collapsed="false" hidden="false" max="15" min="13" style="1" width="8.67611336032389"/>
@@ -3989,15 +3994,15 @@
   <dimension ref="A1:AMC64"/>
   <sheetViews>
     <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="bottomLeft" activeCell="C22" activeCellId="0" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col collapsed="false" hidden="false" max="2" min="1" style="13" width="8.67611336032389"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="13" width="25.8137651821862"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="13" width="26.0283400809717"/>
     <col collapsed="false" hidden="false" max="1017" min="4" style="13" width="8.67611336032389"/>
     <col collapsed="false" hidden="false" max="1025" min="1018" style="0" width="8.67611336032389"/>
   </cols>
@@ -21446,16 +21451,16 @@
   <dimension ref="A1:L22"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G17" activeCellId="0" sqref="G17"/>
+      <selection pane="topLeft" activeCell="F5" activeCellId="0" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col collapsed="false" hidden="false" max="2" min="1" style="0" width="8.67611336032389"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="14.9959514170041"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="15.2105263157895"/>
     <col collapsed="false" hidden="false" max="6" min="4" style="0" width="8.67611336032389"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="13.5263157894737"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="29.6720647773279"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="13.6032388663968"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="30.1012145748988"/>
     <col collapsed="false" hidden="false" max="10" min="9" style="0" width="8.67611336032389"/>
     <col collapsed="false" hidden="false" max="11" min="11" style="0" width="16.3886639676113"/>
     <col collapsed="false" hidden="false" max="1025" min="12" style="0" width="8.67611336032389"/>
@@ -21574,7 +21579,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
         <v>77</v>
       </c>
@@ -21597,7 +21602,7 @@
         <v>225</v>
       </c>
       <c r="H5" s="0" t="s">
-        <v>226</v>
+        <v>200</v>
       </c>
       <c r="K5" s="0" t="s">
         <v>223</v>
@@ -21649,7 +21654,7 @@
         <v>180</v>
       </c>
       <c r="H7" s="0" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="K7" s="0" t="s">
         <v>223</v>
@@ -21704,7 +21709,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
         <v>90</v>
       </c>
@@ -21724,10 +21729,10 @@
         <v>224</v>
       </c>
       <c r="G10" s="0" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="H10" s="0" t="s">
-        <v>196</v>
+        <v>205</v>
       </c>
       <c r="K10" s="0" t="s">
         <v>223</v>
@@ -21756,7 +21761,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
         <v>121</v>
       </c>
@@ -21776,10 +21781,10 @@
         <v>224</v>
       </c>
       <c r="G12" s="0" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="H12" s="0" t="s">
-        <v>196</v>
+        <v>205</v>
       </c>
       <c r="K12" s="0" t="s">
         <v>223</v>
@@ -21802,13 +21807,13 @@
         <v>218</v>
       </c>
       <c r="J13" s="0" t="s">
-        <v>224</v>
+        <v>219</v>
       </c>
       <c r="K13" s="0" t="s">
         <v>220</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
         <v>125</v>
       </c>
@@ -21825,19 +21830,13 @@
         <v>218</v>
       </c>
       <c r="F14" s="0" t="s">
-        <v>224</v>
+        <v>219</v>
       </c>
       <c r="G14" s="0" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="H14" s="0" t="s">
         <v>186</v>
-      </c>
-      <c r="I14" s="0" t="s">
-        <v>218</v>
-      </c>
-      <c r="J14" s="0" t="s">
-        <v>224</v>
       </c>
       <c r="K14" s="0" t="s">
         <v>223</v>
@@ -21935,7 +21934,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
         <v>163</v>
       </c>
@@ -21952,19 +21951,13 @@
         <v>218</v>
       </c>
       <c r="F19" s="0" t="s">
-        <v>224</v>
+        <v>219</v>
       </c>
       <c r="G19" s="0" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="H19" s="0" t="s">
         <v>186</v>
-      </c>
-      <c r="I19" s="0" t="s">
-        <v>218</v>
-      </c>
-      <c r="J19" s="0" t="s">
-        <v>219</v>
       </c>
       <c r="K19" s="0" t="s">
         <v>223</v>
@@ -21993,7 +21986,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
         <v>165</v>
       </c>
@@ -22010,19 +22003,13 @@
         <v>218</v>
       </c>
       <c r="F21" s="0" t="s">
-        <v>224</v>
+        <v>219</v>
       </c>
       <c r="G21" s="0" t="s">
         <v>225</v>
       </c>
       <c r="H21" s="0" t="s">
-        <v>230</v>
-      </c>
-      <c r="I21" s="0" t="s">
-        <v>218</v>
-      </c>
-      <c r="J21" s="0" t="s">
-        <v>219</v>
+        <v>229</v>
       </c>
       <c r="K21" s="0" t="s">
         <v>223</v>
@@ -22069,10 +22056,10 @@
   </sheetPr>
   <dimension ref="A1:J9"/>
   <sheetViews>
-    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="bottomLeft" activeCell="C7" activeCellId="0" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -22081,8 +22068,8 @@
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="13.3886639676113"/>
     <col collapsed="false" hidden="false" max="5" min="4" style="0" width="8.67611336032389"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="0" width="13.9271255060729"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="15.9595141700405"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="12.6396761133603"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="16.1740890688259"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="12.8542510121458"/>
     <col collapsed="false" hidden="false" max="9" min="9" style="0" width="8.67611336032389"/>
     <col collapsed="false" hidden="false" max="10" min="10" style="0" width="13.9271255060729"/>
     <col collapsed="false" hidden="false" max="1025" min="11" style="0" width="8.67611336032389"/>
@@ -22093,7 +22080,7 @@
         <v>2</v>
       </c>
       <c r="B1" s="24" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="C1" s="24" t="s">
         <v>217</v>
@@ -22137,10 +22124,10 @@
         <v>79</v>
       </c>
       <c r="F3" s="0" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="G3" s="0" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="I3" s="0" t="n">
         <v>80</v>
@@ -22151,10 +22138,10 @@
         <v>92</v>
       </c>
       <c r="F4" s="0" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="G4" s="28" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="H4" s="28"/>
       <c r="I4" s="0" t="n">
@@ -22195,7 +22182,7 @@
         <v>27</v>
       </c>
       <c r="F7" s="0" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="G7" s="0" t="s">
         <v>194</v>
@@ -22205,13 +22192,10 @@
       </c>
       <c r="J7" s="29"/>
     </row>
-    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
         <v>99</v>
       </c>
-      <c r="B8" s="0" t="s">
-        <v>219</v>
-      </c>
       <c r="F8" s="0" t="s">
         <v>217</v>
       </c>
@@ -22222,12 +22206,9 @@
         <v>80</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
         <v>141</v>
-      </c>
-      <c r="B9" s="0" t="s">
-        <v>219</v>
       </c>
       <c r="F9" s="0" t="s">
         <v>217</v>
@@ -22275,16 +22256,16 @@
         <v>2</v>
       </c>
       <c r="B1" s="24" t="s">
+        <v>233</v>
+      </c>
+      <c r="C1" s="24" t="s">
         <v>234</v>
       </c>
-      <c r="C1" s="24" t="s">
+      <c r="D1" s="24" t="s">
         <v>235</v>
       </c>
-      <c r="D1" s="24" t="s">
+      <c r="E1" s="24" t="s">
         <v>236</v>
-      </c>
-      <c r="E1" s="24" t="s">
-        <v>237</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -22292,13 +22273,13 @@
         <v>29</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="C2" s="0" t="n">
         <v>114</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -22306,13 +22287,13 @@
         <v>29</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="C3" s="0" t="n">
         <v>120</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -22320,16 +22301,16 @@
         <v>45</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="C4" s="0" t="n">
         <v>86</v>
       </c>
       <c r="D4" s="0" t="s">
+        <v>241</v>
+      </c>
+      <c r="E4" s="0" t="s">
         <v>242</v>
-      </c>
-      <c r="E4" s="0" t="s">
-        <v>243</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -22337,16 +22318,16 @@
         <v>47</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="C5" s="0" t="n">
         <v>86</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -22354,16 +22335,16 @@
         <v>57</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="C6" s="0" t="n">
         <v>86</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -22371,13 +22352,13 @@
         <v>59</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="C7" s="0" t="n">
         <v>83</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -22385,13 +22366,13 @@
         <v>61</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="C8" s="0" t="n">
         <v>84</v>
       </c>
       <c r="D8" s="0" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -22399,13 +22380,13 @@
         <v>63</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="C9" s="0" t="n">
         <v>89</v>
       </c>
       <c r="D9" s="0" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -22413,13 +22394,13 @@
         <v>65</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="C10" s="0" t="n">
         <v>88</v>
       </c>
       <c r="D10" s="0" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -22427,13 +22408,13 @@
         <v>67</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="C11" s="0" t="n">
         <v>85</v>
       </c>
       <c r="D11" s="0" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -22441,16 +22422,16 @@
         <v>69</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="C12" s="0" t="n">
         <v>87</v>
       </c>
       <c r="D12" s="0" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="E12" s="0" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -22458,16 +22439,16 @@
         <v>71</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="C13" s="0" t="n">
         <v>87</v>
       </c>
       <c r="D13" s="0" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="E13" s="0" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -22475,16 +22456,16 @@
         <v>119</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="C14" s="0" t="n">
         <v>98</v>
       </c>
       <c r="D14" s="0" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E14" s="0" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -22492,13 +22473,13 @@
         <v>123</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="C15" s="0" t="n">
         <v>99</v>
       </c>
       <c r="D15" s="0" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -22506,13 +22487,13 @@
         <v>107</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="C16" s="0" t="n">
         <v>123</v>
       </c>
       <c r="D16" s="0" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -22520,16 +22501,16 @@
         <v>108</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="C17" s="0" t="n">
         <v>100</v>
       </c>
       <c r="D17" s="0" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="E17" s="0" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -22537,16 +22518,16 @@
         <v>110</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="C18" s="0" t="n">
         <v>100</v>
       </c>
       <c r="D18" s="0" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="E18" s="0" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -22554,16 +22535,16 @@
         <v>112</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="C19" s="0" t="n">
         <v>98</v>
       </c>
       <c r="D19" s="0" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="E19" s="0" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -22571,13 +22552,13 @@
         <v>168</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="C20" s="0" t="n">
         <v>123</v>
       </c>
       <c r="D20" s="0" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -22585,13 +22566,13 @@
         <v>148</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="C21" s="0" t="n">
         <v>110</v>
       </c>
       <c r="D21" s="0" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -22599,16 +22580,16 @@
         <v>150</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="C22" s="0" t="n">
         <v>118</v>
       </c>
       <c r="D22" s="0" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="E22" s="0" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -22616,16 +22597,16 @@
         <v>152</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="C23" s="0" t="n">
         <v>118</v>
       </c>
       <c r="D23" s="0" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="E23" s="0" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -22633,16 +22614,16 @@
         <v>154</v>
       </c>
       <c r="B24" s="0" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="C24" s="0" t="n">
         <v>118</v>
       </c>
       <c r="D24" s="0" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="E24" s="0" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
   </sheetData>
@@ -22693,7 +22674,7 @@
         <v>179</v>
       </c>
       <c r="F1" s="24" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -22701,7 +22682,7 @@
         <v>87</v>
       </c>
       <c r="F2" s="0" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
     </row>
   </sheetData>
@@ -22733,47 +22714,47 @@
   <sheetData>
     <row r="1" s="24" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="24" t="s">
+        <v>268</v>
+      </c>
+      <c r="B1" s="24" t="s">
         <v>269</v>
-      </c>
-      <c r="B1" s="24" t="s">
-        <v>270</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
+        <v>270</v>
+      </c>
+      <c r="B2" s="0" t="s">
         <v>271</v>
-      </c>
-      <c r="B2" s="0" t="s">
-        <v>272</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
+        <v>273</v>
+      </c>
+      <c r="B4" s="0" t="s">
         <v>274</v>
-      </c>
-      <c r="B4" s="0" t="s">
-        <v>275</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
+        <v>275</v>
+      </c>
+      <c r="B5" s="0" t="s">
         <v>276</v>
-      </c>
-      <c r="B5" s="0" t="s">
-        <v>277</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="B6" s="0" t="s">
         <v>218</v>
@@ -22781,7 +22762,7 @@
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="B7" s="0" t="s">
         <v>217</v>
@@ -22789,7 +22770,7 @@
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="B8" s="0" t="s">
         <v>218</v>
@@ -22805,10 +22786,10 @@
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>